<commit_message>
test complex modal and implement the operation of single question (moveUp, moveDown, remove)
</commit_message>
<xml_diff>
--- a/doc/迭代开发计划_whyNotDance.xlsx
+++ b/doc/迭代开发计划_whyNotDance.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26215"/>
+  <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wang-cy/Desktop/prj1_whynotdance/doc/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16000" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Use Cases" sheetId="2" r:id="rId1"/>
@@ -14,12 +19,17 @@
     <sheet name="Sprint 3" sheetId="5" r:id="rId5"/>
     <sheet name="Sprint 4" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="104">
   <si>
     <t>Feature_ID</t>
   </si>
@@ -405,6 +415,168 @@
   </si>
   <si>
     <t>作为一个发布者，测试代码的利用率</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC_2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>信息收集和管理</t>
+    <rPh sb="0" eb="1">
+      <t>xin'xi'shou'ji</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>he</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>guan'li</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>活动发布者可以通过链接发布问卷，之后可以查看、查询、筛选，并导出数据。活动参与者通过链接填写问卷，后台数据库实时更新</t>
+    <rPh sb="0" eb="1">
+      <t>huo'dong'fa'bu'zhe</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>zhe</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>ke'yi</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>tong'guo</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>lian'jie</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>fa'bu</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>wen'juan</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>zhi'hou</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>ke'yi</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>cha'kan</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>cha'xun</t>
+    </rPh>
+    <rPh sb="26" eb="27">
+      <t>shai'xuan</t>
+    </rPh>
+    <rPh sb="29" eb="30">
+      <t>bing</t>
+    </rPh>
+    <rPh sb="30" eb="31">
+      <t>dao'chu</t>
+    </rPh>
+    <rPh sb="32" eb="33">
+      <t>shu'ju</t>
+    </rPh>
+    <rPh sb="35" eb="36">
+      <t>huo'dong</t>
+    </rPh>
+    <rPh sb="37" eb="38">
+      <t>cna'yu'zhe</t>
+    </rPh>
+    <rPh sb="40" eb="41">
+      <t>tong'guo</t>
+    </rPh>
+    <rPh sb="42" eb="43">
+      <t>lian'jie</t>
+    </rPh>
+    <rPh sb="44" eb="45">
+      <t>tian'xie'wen'juan</t>
+    </rPh>
+    <rPh sb="49" eb="50">
+      <t>hou'tai</t>
+    </rPh>
+    <rPh sb="51" eb="52">
+      <t>shu'ju'ku</t>
+    </rPh>
+    <rPh sb="54" eb="55">
+      <t>shi'shi'geng'xin</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC_3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据整理、分析、可视化</t>
+    <rPh sb="0" eb="1">
+      <t>shu'ju</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>zheng'li</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>fen'xi</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>ke'shi'hua</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>活动发布者可以查看不同ip的输入信息，并对数据进行简单的分析，可以导出原始数据和分析结果</t>
+    <rPh sb="0" eb="1">
+      <t>huo'dong'fa'bu'zhe</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>ke'yi</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>cha'kan</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>bu'tong</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>de</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>shu'ru</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>xin'xi</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>bing'dui</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>shu'ju</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>jin'xing</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>jian'dan</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>de</t>
+    </rPh>
+    <rPh sb="28" eb="29">
+      <t>fen'xi</t>
+    </rPh>
+    <rPh sb="35" eb="36">
+      <t>yuan'shi'shu'ju</t>
+    </rPh>
+    <rPh sb="39" eb="40">
+      <t>he</t>
+    </rPh>
+    <rPh sb="40" eb="41">
+      <t>fen'xi'jie'guo</t>
+    </rPh>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -787,17 +959,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="19.75" customWidth="1"/>
-    <col min="2" max="2" width="24.75" customWidth="1"/>
-    <col min="3" max="3" width="97.25" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" customWidth="1"/>
+    <col min="3" max="3" width="111.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.15">
@@ -820,6 +992,28 @@
       </c>
       <c r="C2" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -832,21 +1026,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="125" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="14.625" customWidth="1"/>
-    <col min="2" max="2" width="14.75" customWidth="1"/>
-    <col min="3" max="3" width="16.625" customWidth="1"/>
-    <col min="4" max="4" width="15.125" customWidth="1"/>
-    <col min="5" max="5" width="108.75" customWidth="1"/>
+    <col min="1" max="2" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" customWidth="1"/>
+    <col min="5" max="5" width="108.6640625" customWidth="1"/>
     <col min="6" max="6" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1030,18 +1223,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="15.75" customWidth="1"/>
-    <col min="2" max="2" width="30.75" customWidth="1"/>
-    <col min="3" max="3" width="14.625" customWidth="1"/>
-    <col min="4" max="4" width="19.25" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="19.1640625" customWidth="1"/>
     <col min="5" max="5" width="20.5" customWidth="1"/>
-    <col min="6" max="6" width="19.875" customWidth="1"/>
+    <col min="6" max="6" width="19.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.15">
@@ -1153,6 +1346,9 @@
       <c r="C7" t="s">
         <v>24</v>
       </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
@@ -1164,6 +1360,9 @@
       <c r="C8" t="s">
         <v>80</v>
       </c>
+      <c r="D8">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
@@ -1203,6 +1402,9 @@
       <c r="C11" t="s">
         <v>89</v>
       </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
@@ -1242,6 +1444,9 @@
       <c r="C14" t="s">
         <v>90</v>
       </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
@@ -1256,6 +1461,9 @@
       <c r="D15">
         <v>3</v>
       </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
@@ -1334,6 +1542,9 @@
       </c>
       <c r="C20" t="s">
         <v>80</v>
+      </c>
+      <c r="D20">
+        <v>1.5</v>
       </c>
     </row>
   </sheetData>
@@ -1350,14 +1561,14 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="14.375" customWidth="1"/>
-    <col min="2" max="2" width="17.875" customWidth="1"/>
-    <col min="3" max="3" width="12.875" customWidth="1"/>
-    <col min="4" max="4" width="19.875" customWidth="1"/>
-    <col min="5" max="5" width="18.375" customWidth="1"/>
-    <col min="6" max="6" width="17.375" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" customWidth="1"/>
+    <col min="4" max="4" width="19.83203125" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.15">
@@ -1394,7 +1605,7 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.125" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.1640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
@@ -1430,7 +1641,7 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="19.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">

</xml_diff>

<commit_message>
modify api and corresponding doc
</commit_message>
<xml_diff>
--- a/doc/迭代开发计划_whyNotDance.xlsx
+++ b/doc/迭代开发计划_whyNotDance.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16000" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Use Cases" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="174">
   <si>
     <t>Feature_ID</t>
   </si>
@@ -1795,6 +1795,946 @@
   </si>
   <si>
     <t>F_26</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F_27</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>登录界面表单提交到数据库</t>
+    <rPh sb="0" eb="1">
+      <t>deng'lu'jie'mian</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>biao'dan</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>ti'jiao</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>dao</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>shu'ju'ku</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F_28</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>个人信息修改提交到数据库</t>
+    <rPh sb="0" eb="1">
+      <t>ge'ren</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>xin'xi</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>xiu'gai</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>ti'jiao'dao</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>shu'ju'ku</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F_29</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>游客主界面设计</t>
+    <rPh sb="0" eb="1">
+      <t>you'ke'jia'mian</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>zhu</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>she'ji</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F_30</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>超级管理员主界面设计</t>
+    <rPh sb="0" eb="1">
+      <t>chao'ji'guan'li'yuan</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>zhu'jie'mian</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>she'ji</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>田文龙</t>
+    <rPh sb="0" eb="1">
+      <t>tian'wen'long</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F_31</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>发布出的问卷页面设计</t>
+    <rPh sb="0" eb="1">
+      <t>fa'bu</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>chu</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>de</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>wen'jua</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>ye'mian</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>she'ji</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F_32</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>问卷保存和发布向后端发送消息</t>
+    <rPh sb="0" eb="1">
+      <t>wen'juan</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>bao'cun</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>he</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>fa'bu</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>xiang</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>hou'duan</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>fa'song'xiao'xi</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F_33</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>多选题页面设计</t>
+    <rPh sb="0" eb="1">
+      <t>duo'xuan'ti</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ye'mian'she'ji</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F_34</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>多选题在线编辑并提交修改到后端</t>
+    <rPh sb="0" eb="1">
+      <t>duo'xuan'ti</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>zai'xian'bian'ji</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>bing</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>ti'jiao'xiu'gai</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>dao</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>hou'duan</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>王晨阳</t>
+    <rPh sb="0" eb="1">
+      <t>wang'chen'ayng</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F_35</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>填空题具体实现</t>
+    <rPh sb="0" eb="1">
+      <t>tian'kong'ti</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ju'ti'shi'xian</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F_36</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>修改问卷页面跳转和实现</t>
+    <rPh sb="0" eb="1">
+      <t>xiu'gai'wen'juan</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>ye'mian</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>tiao'zhuan</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>he</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>shi'xian</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F_37</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据库响应删除问卷操作</t>
+    <rPh sb="0" eb="1">
+      <t>shu'ju'ku'xiang'ying</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>xiang'ying</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>shan'chu'wen'juan</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>cao'zuo</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>徐子南</t>
+    <rPh sb="0" eb="1">
+      <t>xu'zi'nan</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F_38</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据库保存对题目的操作</t>
+    <rPh sb="0" eb="1">
+      <t>shu'ju'ku</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>bao'cun</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>dui</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>ti'mu</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>de</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>cao'zuo</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F_39</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据库保存对问卷题目和说明的编辑</t>
+    <rPh sb="0" eb="1">
+      <t>shu'ju'ku</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>bao'cun</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>dui'wen'juan</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>ti'mu</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>he</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>shuo'ming</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>de</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>bian'ji</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC_2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>作为一个用户，可以在登录界面输入账号密码，后台进行验证</t>
+    <rPh sb="0" eb="1">
+      <t>zuo'wei'yi'ge</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>yong'hu</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>ke'yi'zai</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>zai</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>deng'lu'jie'mian</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>shu'ru</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>zhang'hao'mi'ma</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>hou'tai</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>jin'xing'yan'zheng</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>作为一个已注册用户，可以在个人信息修改页面修改信息，网页实时更新，并把修改内容提交到数据库</t>
+    <rPh sb="0" eb="1">
+      <t>zuo'wei'yi'ge</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>yi'zhu'ce</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>yong'hu</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>ke'yi</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>zai</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>ge'ren'xin'xi</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>xiu'gai</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>ye'mian</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>xiu'gai</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>xin'xi</t>
+    </rPh>
+    <rPh sb="26" eb="27">
+      <t>wang'ye</t>
+    </rPh>
+    <rPh sb="28" eb="29">
+      <t>shi'shi</t>
+    </rPh>
+    <rPh sb="30" eb="31">
+      <t>geng'xin</t>
+    </rPh>
+    <rPh sb="33" eb="34">
+      <t>bing</t>
+    </rPh>
+    <rPh sb="34" eb="35">
+      <t>ba</t>
+    </rPh>
+    <rPh sb="35" eb="36">
+      <t>xiu'gai</t>
+    </rPh>
+    <rPh sb="37" eb="38">
+      <t>nei'rong</t>
+    </rPh>
+    <rPh sb="39" eb="40">
+      <t>ti'jiao'dao</t>
+    </rPh>
+    <rPh sb="42" eb="43">
+      <t>shu'ju'ku</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>作为一个超级管理员，输入账号密码登陆后可以看到超级管理员的主界面，包括管理注册用户和发布公告等功能</t>
+    <rPh sb="0" eb="1">
+      <t>zuo'wei'yi'ge</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>chao'ji'guan'li'yuan</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>shu'ru</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>zhang'hao'mi'ma</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>deng'lu'hou</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>ke'yi'kan'dao</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>chao'ji'guan'li'yuan'de</t>
+    </rPh>
+    <rPh sb="29" eb="30">
+      <t>zhu'jie'mian</t>
+    </rPh>
+    <rPh sb="33" eb="34">
+      <t>bao'kuo</t>
+    </rPh>
+    <rPh sb="35" eb="36">
+      <t>guan'li</t>
+    </rPh>
+    <rPh sb="37" eb="38">
+      <t>zhu'ce'yong'hu</t>
+    </rPh>
+    <rPh sb="41" eb="42">
+      <t>he</t>
+    </rPh>
+    <rPh sb="42" eb="43">
+      <t>fa'bu'gong'gao</t>
+    </rPh>
+    <rPh sb="46" eb="47">
+      <t>deng'gong'neng</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>作为一个活动参与者，可以点击问卷链接看到问卷的内容</t>
+    <rPh sb="0" eb="1">
+      <t>zuo'wei'yi'ge</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>huo'dong</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>can'yu'zhe</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>ke'yi'dian'ji</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>wen'juan'lian'jie</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>kan'dao</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>wen'juan'de</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>nei'rong</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>作为一个游客，直接登录网站可以看到游客界面</t>
+    <rPh sb="0" eb="1">
+      <t>zuo'wei'yi'ge</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>you'ke</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>zhi'jie</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>deng'lu</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>wang'zhan</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>ke'yi'kan'dao</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>you'ke'jie'mian</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>作为一个用户，设计问卷之后点击保存按钮向后端发送消息修改问卷状态；发布时同理</t>
+    <rPh sb="0" eb="1">
+      <t>zuo'wei'yi'ge</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>yong'hu</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>she'ji'wen'juan'zhi'hou</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>dian'ji</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>bao'cun</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>an'niu</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>xiang'hou'duan</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>fa'song'xiao'xi</t>
+    </rPh>
+    <rPh sb="26" eb="27">
+      <t>xiu'gai'wen'juan'zhuang'tai</t>
+    </rPh>
+    <rPh sb="33" eb="34">
+      <t>fa'bu'shi</t>
+    </rPh>
+    <rPh sb="36" eb="37">
+      <t>tong'li</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>作为一个用户，可以再设计问卷页面点击多选题类型在问卷中添加多选题</t>
+    <rPh sb="0" eb="1">
+      <t>zuo'wei</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>yi'ge</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>yong'hu</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>ke'yi</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>zai</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>she'ji'wen'juan</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>ye'mian</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>dian'ji</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>duo'xuan'ti</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>lei'xing</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>zai</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>wen'juan'zhong</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>tian'jia</t>
+    </rPh>
+    <rPh sb="29" eb="30">
+      <t>duo'xuan'ti</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>作为一个用户，点击多选题的“编辑”按钮后，可以在线修改，网页实时更新，并提交修改到后端保存</t>
+    <rPh sb="0" eb="1">
+      <t>zuo'wei'yi'ge</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>yong'hu</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>dian'ji</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>duo'xuan'ti</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>de</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>bian'ji</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>an'niu'hou</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>ke'yi</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>zai'xian</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>xiu'gai</t>
+    </rPh>
+    <rPh sb="28" eb="29">
+      <t>wang'ye</t>
+    </rPh>
+    <rPh sb="30" eb="31">
+      <t>shi'shi</t>
+    </rPh>
+    <rPh sb="32" eb="33">
+      <t>geng'xin</t>
+    </rPh>
+    <rPh sb="35" eb="36">
+      <t>bing</t>
+    </rPh>
+    <rPh sb="36" eb="37">
+      <t>ti'jiao</t>
+    </rPh>
+    <rPh sb="38" eb="39">
+      <t>xiu'gai'dao</t>
+    </rPh>
+    <rPh sb="41" eb="42">
+      <t>hou'duan</t>
+    </rPh>
+    <rPh sb="43" eb="44">
+      <t>bao'cun</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>作为一个用户，可以选择填空题题型，并在线编辑题目，保存之后提交修改到数据库</t>
+    <rPh sb="0" eb="1">
+      <t>zuo'wei'yi'ge</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>yong'hu</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>ke'yi</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>xuan'ze</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>tian'kong'ti</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>ti'xing</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>bing</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>zai'xian'bia'ji</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>ti'mu</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>bao'cun'zhi'hou</t>
+    </rPh>
+    <rPh sb="29" eb="30">
+      <t>ti'jiao</t>
+    </rPh>
+    <rPh sb="31" eb="32">
+      <t>xiu'gai'dao</t>
+    </rPh>
+    <rPh sb="34" eb="35">
+      <t>shu'ju'ku</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>作为一个已注册用户，可以再待发布问卷的操作中选择修改，并跳转到对应的修改页面，页面包含已有的题目</t>
+    <rPh sb="0" eb="1">
+      <t>zuo'wei'yi'ge</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>yi'zhu'ce</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>yong'hu</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>ke'yi</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>zai</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>dai'fa'bu'wen'juan'de</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>cao'zuo'zhong</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>xuan'ze</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>xiu'ga</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>bing</t>
+    </rPh>
+    <rPh sb="28" eb="29">
+      <t>tiao'zhuan'dao</t>
+    </rPh>
+    <rPh sb="31" eb="32">
+      <t>dui'ying'de</t>
+    </rPh>
+    <rPh sb="34" eb="35">
+      <t>xiu'gai'ye'mai</t>
+    </rPh>
+    <rPh sb="36" eb="37">
+      <t>ye'mian</t>
+    </rPh>
+    <rPh sb="39" eb="40">
+      <t>ye'mian</t>
+    </rPh>
+    <rPh sb="41" eb="42">
+      <t>bao'han</t>
+    </rPh>
+    <rPh sb="43" eb="44">
+      <t>yi</t>
+    </rPh>
+    <rPh sb="44" eb="45">
+      <t>you</t>
+    </rPh>
+    <rPh sb="45" eb="46">
+      <t>de</t>
+    </rPh>
+    <rPh sb="46" eb="47">
+      <t>ti'mu</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>作为一个用户，在对每个问卷的操作中点击“删除”后，前端发送包括问卷id的消息，数据库将相应问卷标为已删除</t>
+    <rPh sb="0" eb="1">
+      <t>zuo'wei'yi'ge</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>yong'hu</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>zai</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>dui</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>mei'ge</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>wen'juan'de</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>cao'zuo</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>zhong</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>dian'ji</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>shan'chu</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>hou</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>qian'duan</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>fa'song'bao'kuo</t>
+    </rPh>
+    <rPh sb="31" eb="32">
+      <t>wen'juan</t>
+    </rPh>
+    <rPh sb="35" eb="36">
+      <t>de</t>
+    </rPh>
+    <rPh sb="36" eb="37">
+      <t>xiao'xi</t>
+    </rPh>
+    <rPh sb="39" eb="40">
+      <t>shu'ju'ku</t>
+    </rPh>
+    <rPh sb="42" eb="43">
+      <t>jiang</t>
+    </rPh>
+    <rPh sb="43" eb="44">
+      <t>xiang'ying'wen'juan</t>
+    </rPh>
+    <rPh sb="47" eb="48">
+      <t>biao'wei</t>
+    </rPh>
+    <rPh sb="49" eb="50">
+      <t>yi'shan'chu</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>作为一个用户，点击对题目的操作后向后端发送消息，后端根据操作的类型进行数据库相应操作</t>
+    <rPh sb="0" eb="1">
+      <t>zuo'wei'yi'ge'yong'hu</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>dian'ji</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>dui'ti'mu</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>de</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>cao'zuo</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>hou</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>xiang</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>hou'duan</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>fa'song</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>xiao'xi</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>hou'duan'gen'ju</t>
+    </rPh>
+    <rPh sb="28" eb="29">
+      <t>cao'zuo'de</t>
+    </rPh>
+    <rPh sb="31" eb="32">
+      <t>lei'xing</t>
+    </rPh>
+    <rPh sb="33" eb="34">
+      <t>jing'xing</t>
+    </rPh>
+    <rPh sb="35" eb="36">
+      <t>shu'ju'ku</t>
+    </rPh>
+    <rPh sb="38" eb="39">
+      <t>xiang'ying</t>
+    </rPh>
+    <rPh sb="40" eb="41">
+      <t>cao'zuo</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>作为一个用户，可以在弹出的模态框中在线编辑问卷题目和说明，点击保存后数据库更新问卷题目和说明</t>
+    <rPh sb="0" eb="1">
+      <t>zuo'wei'yi'ge</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>yong'hu</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>ke'yi'zai'xian</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>zai</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>tan'chu</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>de</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>mo'tai'kuang'zhong</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>bian'ji</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>wen'juan</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>ti'mu</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>he</t>
+    </rPh>
+    <rPh sb="26" eb="27">
+      <t>hsuo'ming</t>
+    </rPh>
+    <rPh sb="29" eb="30">
+      <t>dian'ji</t>
+    </rPh>
+    <rPh sb="31" eb="32">
+      <t>bao'cun'hou</t>
+    </rPh>
+    <rPh sb="34" eb="35">
+      <t>shu'ju'ku</t>
+    </rPh>
+    <rPh sb="37" eb="38">
+      <t>geng'xin</t>
+    </rPh>
+    <rPh sb="39" eb="40">
+      <t>wen'juan</t>
+    </rPh>
+    <rPh sb="41" eb="42">
+      <t>ti'mu</t>
+    </rPh>
+    <rPh sb="43" eb="44">
+      <t>he</t>
+    </rPh>
+    <rPh sb="44" eb="45">
+      <t>shu'oing</t>
+    </rPh>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -2242,10 +3182,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="A27" sqref="A2:A27"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -2719,6 +3659,227 @@
         <v>112</v>
       </c>
     </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A28" t="s">
+        <v>131</v>
+      </c>
+      <c r="B28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" t="s">
+        <v>132</v>
+      </c>
+      <c r="D28" t="s">
+        <v>75</v>
+      </c>
+      <c r="E28" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A29" t="s">
+        <v>133</v>
+      </c>
+      <c r="B29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" t="s">
+        <v>134</v>
+      </c>
+      <c r="D29" t="s">
+        <v>75</v>
+      </c>
+      <c r="E29" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A30" t="s">
+        <v>135</v>
+      </c>
+      <c r="B30" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" t="s">
+        <v>136</v>
+      </c>
+      <c r="D30" t="s">
+        <v>75</v>
+      </c>
+      <c r="E30" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A31" t="s">
+        <v>137</v>
+      </c>
+      <c r="B31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" t="s">
+        <v>138</v>
+      </c>
+      <c r="D31" t="s">
+        <v>139</v>
+      </c>
+      <c r="E31" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A32" t="s">
+        <v>140</v>
+      </c>
+      <c r="B32" t="s">
+        <v>160</v>
+      </c>
+      <c r="C32" t="s">
+        <v>141</v>
+      </c>
+      <c r="D32" t="s">
+        <v>139</v>
+      </c>
+      <c r="E32" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A33" t="s">
+        <v>142</v>
+      </c>
+      <c r="B33" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" t="s">
+        <v>143</v>
+      </c>
+      <c r="D33" t="s">
+        <v>82</v>
+      </c>
+      <c r="E33" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A34" t="s">
+        <v>144</v>
+      </c>
+      <c r="B34" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" t="s">
+        <v>145</v>
+      </c>
+      <c r="D34" t="s">
+        <v>82</v>
+      </c>
+      <c r="E34" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A35" t="s">
+        <v>146</v>
+      </c>
+      <c r="B35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" t="s">
+        <v>147</v>
+      </c>
+      <c r="D35" t="s">
+        <v>148</v>
+      </c>
+      <c r="E35" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A36" t="s">
+        <v>149</v>
+      </c>
+      <c r="B36" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" t="s">
+        <v>150</v>
+      </c>
+      <c r="D36" t="s">
+        <v>82</v>
+      </c>
+      <c r="E36" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A37" t="s">
+        <v>151</v>
+      </c>
+      <c r="B37" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" t="s">
+        <v>152</v>
+      </c>
+      <c r="D37" t="s">
+        <v>82</v>
+      </c>
+      <c r="E37" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A38" t="s">
+        <v>153</v>
+      </c>
+      <c r="B38" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" t="s">
+        <v>154</v>
+      </c>
+      <c r="D38" t="s">
+        <v>155</v>
+      </c>
+      <c r="E38" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A39" t="s">
+        <v>156</v>
+      </c>
+      <c r="B39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" t="s">
+        <v>157</v>
+      </c>
+      <c r="D39" t="s">
+        <v>155</v>
+      </c>
+      <c r="E39" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A40" t="s">
+        <v>158</v>
+      </c>
+      <c r="B40" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" t="s">
+        <v>159</v>
+      </c>
+      <c r="D40" t="s">
+        <v>155</v>
+      </c>
+      <c r="E40" t="s">
+        <v>173</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2728,10 +3889,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A27" sqref="A2:A27"/>
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -2777,6 +3938,9 @@
       <c r="D2">
         <v>3</v>
       </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
@@ -2856,6 +4020,9 @@
       <c r="D7">
         <v>2</v>
       </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
@@ -2870,6 +4037,9 @@
       <c r="D8">
         <v>0.5</v>
       </c>
+      <c r="E8">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
@@ -2915,6 +4085,9 @@
       <c r="D11">
         <v>1</v>
       </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
@@ -3171,6 +4344,188 @@
       </c>
       <c r="E27">
         <v>0.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A28" t="s">
+        <v>131</v>
+      </c>
+      <c r="B28" t="s">
+        <v>132</v>
+      </c>
+      <c r="C28" t="s">
+        <v>75</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A29" t="s">
+        <v>133</v>
+      </c>
+      <c r="B29" t="s">
+        <v>134</v>
+      </c>
+      <c r="C29" t="s">
+        <v>75</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A30" t="s">
+        <v>135</v>
+      </c>
+      <c r="B30" t="s">
+        <v>136</v>
+      </c>
+      <c r="C30" t="s">
+        <v>75</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A31" t="s">
+        <v>137</v>
+      </c>
+      <c r="B31" t="s">
+        <v>138</v>
+      </c>
+      <c r="C31" t="s">
+        <v>139</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A32" t="s">
+        <v>140</v>
+      </c>
+      <c r="B32" t="s">
+        <v>141</v>
+      </c>
+      <c r="C32" t="s">
+        <v>139</v>
+      </c>
+      <c r="D32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A33" t="s">
+        <v>142</v>
+      </c>
+      <c r="B33" t="s">
+        <v>143</v>
+      </c>
+      <c r="C33" t="s">
+        <v>82</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A34" t="s">
+        <v>144</v>
+      </c>
+      <c r="B34" t="s">
+        <v>145</v>
+      </c>
+      <c r="C34" t="s">
+        <v>82</v>
+      </c>
+      <c r="D34">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A35" t="s">
+        <v>146</v>
+      </c>
+      <c r="B35" t="s">
+        <v>147</v>
+      </c>
+      <c r="C35" t="s">
+        <v>148</v>
+      </c>
+      <c r="D35">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A36" t="s">
+        <v>149</v>
+      </c>
+      <c r="B36" t="s">
+        <v>150</v>
+      </c>
+      <c r="C36" t="s">
+        <v>82</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A37" t="s">
+        <v>151</v>
+      </c>
+      <c r="B37" t="s">
+        <v>152</v>
+      </c>
+      <c r="C37" t="s">
+        <v>82</v>
+      </c>
+      <c r="D37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A38" t="s">
+        <v>153</v>
+      </c>
+      <c r="B38" t="s">
+        <v>154</v>
+      </c>
+      <c r="C38" t="s">
+        <v>155</v>
+      </c>
+      <c r="D38">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A39" t="s">
+        <v>156</v>
+      </c>
+      <c r="B39" t="s">
+        <v>157</v>
+      </c>
+      <c r="C39" t="s">
+        <v>155</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A40" t="s">
+        <v>158</v>
+      </c>
+      <c r="B40" t="s">
+        <v>159</v>
+      </c>
+      <c r="C40" t="s">
+        <v>155</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
improve the appearence of radio button and fix some id bugs which can lead to wrong direction when click the lable of an option
</commit_message>
<xml_diff>
--- a/doc/迭代开发计划_whyNotDance.xlsx
+++ b/doc/迭代开发计划_whyNotDance.xlsx
@@ -3232,7 +3232,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="14.1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -3249,7 +3249,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -3266,7 +3266,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="14.1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -3283,7 +3283,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="14.1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -3300,7 +3300,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="14.1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -3317,7 +3317,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="14.1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -3334,7 +3334,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="14.1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -3351,7 +3351,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="14.1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>48</v>
       </c>
@@ -3368,7 +3368,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="14.1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>64</v>
       </c>
@@ -3385,7 +3385,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="14.1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>114</v>
       </c>
@@ -3402,7 +3402,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="14.1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>115</v>
       </c>
@@ -3419,7 +3419,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="14.1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>116</v>
       </c>
@@ -3436,7 +3436,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="14.1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>117</v>
       </c>
@@ -3453,7 +3453,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="14.1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>118</v>
       </c>
@@ -3470,7 +3470,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="14.1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>119</v>
       </c>
@@ -3487,7 +3487,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="14.1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>120</v>
       </c>
@@ -3504,7 +3504,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="14.1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>121</v>
       </c>
@@ -3521,7 +3521,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="14.1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>122</v>
       </c>
@@ -3538,7 +3538,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="14.1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>123</v>
       </c>
@@ -3555,7 +3555,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="14.1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>124</v>
       </c>
@@ -3572,7 +3572,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="14.1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>125</v>
       </c>
@@ -3589,7 +3589,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="14.1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>126</v>
       </c>
@@ -3906,8 +3906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4068,6 +4068,9 @@
       </c>
       <c r="D9">
         <v>3</v>
+      </c>
+      <c r="E9">
+        <v>1.5</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
add multi questions and fillin questions
</commit_message>
<xml_diff>
--- a/doc/迭代开发计划_whyNotDance.xlsx
+++ b/doc/迭代开发计划_whyNotDance.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26215"/>
+  <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wang-cy/Desktop/prj1_whynotdance/doc/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="15945" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Use Cases" sheetId="2" r:id="rId1"/>
@@ -24,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="185">
   <si>
     <t>Feature_ID</t>
   </si>
@@ -85,10 +90,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>活动发布设计</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>徐子南</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -129,10 +130,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>用户登录网站，设计报名表，发布主观问答、选择等题目，对题目进行编辑处理，以链接形式发布问卷</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>F_1</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -298,96 +295,6 @@
   </si>
   <si>
     <t>UC_2</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>信息收集和管理</t>
-    <rPh sb="0" eb="1">
-      <t>xin'xi'shou'ji</t>
-    </rPh>
-    <rPh sb="4" eb="5">
-      <t>he</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>guan'li</t>
-    </rPh>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>活动发布者可以通过链接发布问卷，之后可以查看、查询、筛选，并导出数据。活动参与者通过链接填写问卷，后台数据库实时更新</t>
-    <rPh sb="0" eb="1">
-      <t>huo'dong'fa'bu'zhe</t>
-    </rPh>
-    <rPh sb="4" eb="5">
-      <t>zhe</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>ke'yi</t>
-    </rPh>
-    <rPh sb="7" eb="8">
-      <t>tong'guo</t>
-    </rPh>
-    <rPh sb="9" eb="10">
-      <t>lian'jie</t>
-    </rPh>
-    <rPh sb="11" eb="12">
-      <t>fa'bu</t>
-    </rPh>
-    <rPh sb="13" eb="14">
-      <t>wen'juan</t>
-    </rPh>
-    <rPh sb="16" eb="17">
-      <t>zhi'hou</t>
-    </rPh>
-    <rPh sb="18" eb="19">
-      <t>ke'yi</t>
-    </rPh>
-    <rPh sb="20" eb="21">
-      <t>cha'kan</t>
-    </rPh>
-    <rPh sb="23" eb="24">
-      <t>cha'xun</t>
-    </rPh>
-    <rPh sb="26" eb="27">
-      <t>shai'xuan</t>
-    </rPh>
-    <rPh sb="29" eb="30">
-      <t>bing</t>
-    </rPh>
-    <rPh sb="30" eb="31">
-      <t>dao'chu</t>
-    </rPh>
-    <rPh sb="32" eb="33">
-      <t>shu'ju</t>
-    </rPh>
-    <rPh sb="35" eb="36">
-      <t>huo'dong</t>
-    </rPh>
-    <rPh sb="37" eb="38">
-      <t>cna'yu'zhe</t>
-    </rPh>
-    <rPh sb="40" eb="41">
-      <t>tong'guo</t>
-    </rPh>
-    <rPh sb="42" eb="43">
-      <t>lian'jie</t>
-    </rPh>
-    <rPh sb="44" eb="45">
-      <t>tian'xie'wen'juan</t>
-    </rPh>
-    <rPh sb="49" eb="50">
-      <t>hou'tai</t>
-    </rPh>
-    <rPh sb="51" eb="52">
-      <t>shu'ju'ku</t>
-    </rPh>
-    <rPh sb="54" eb="55">
-      <t>shi'shi'geng'xin</t>
-    </rPh>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>UC_3</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -403,58 +310,6 @@
     </rPh>
     <rPh sb="8" eb="9">
       <t>ke'shi'hua</t>
-    </rPh>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>活动发布者可以查看不同ip的输入信息，并对数据进行简单的分析，可以导出原始数据和分析结果</t>
-    <rPh sb="0" eb="1">
-      <t>huo'dong'fa'bu'zhe</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>ke'yi</t>
-    </rPh>
-    <rPh sb="7" eb="8">
-      <t>cha'kan</t>
-    </rPh>
-    <rPh sb="9" eb="10">
-      <t>bu'tong</t>
-    </rPh>
-    <rPh sb="13" eb="14">
-      <t>de</t>
-    </rPh>
-    <rPh sb="14" eb="15">
-      <t>shu'ru</t>
-    </rPh>
-    <rPh sb="16" eb="17">
-      <t>xin'xi</t>
-    </rPh>
-    <rPh sb="19" eb="20">
-      <t>bing'dui</t>
-    </rPh>
-    <rPh sb="21" eb="22">
-      <t>shu'ju</t>
-    </rPh>
-    <rPh sb="23" eb="24">
-      <t>jin'xing</t>
-    </rPh>
-    <rPh sb="25" eb="26">
-      <t>jian'dan</t>
-    </rPh>
-    <rPh sb="27" eb="28">
-      <t>de</t>
-    </rPh>
-    <rPh sb="28" eb="29">
-      <t>fen'xi</t>
-    </rPh>
-    <rPh sb="35" eb="36">
-      <t>yuan'shi'shu'ju</t>
-    </rPh>
-    <rPh sb="39" eb="40">
-      <t>he</t>
-    </rPh>
-    <rPh sb="40" eb="41">
-      <t>fen'xi'jie'guo</t>
     </rPh>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -2750,6 +2605,225 @@
   </si>
   <si>
     <t>王晨阳</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC_3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>信息概览及活动设计</t>
+    <rPh sb="0" eb="1">
+      <t>xin'xi'gai'lan</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>ji</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>活动发布和管理</t>
+    <rPh sb="0" eb="1">
+      <t>huo'dong'fa'bu</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>he</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>guan'li</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>活动参与和信息收集</t>
+    <rPh sb="0" eb="1">
+      <t>huo'dong</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>can'yu</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>he</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>xin'xi'shou'ji</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>活动发布者可以通过链接发布问卷，之后可以查看、查询。</t>
+    <rPh sb="0" eb="1">
+      <t>huo'dong'fa'bu'zhe</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>zhe</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>ke'yi</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>tong'guo</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>lian'jie</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>fa'bu</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>wen'juan</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>zhi'hou</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>ke'yi</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>cha'kan</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>cha'xun</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC_4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户登录网站，设计报名表，发布主观问答、选择等题目，对题目进行编辑处理。</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>活动参与者通过链接填写问卷，后台数据库实时更新。</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>活动发布者可以查看不同ip的输入信息，并对数据进行简单的分析，可以导出原始数据和分析结果。</t>
+    <rPh sb="0" eb="1">
+      <t>huo'dong'fa'bu'zhe</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>ke'yi</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>cha'kan</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>bu'tong</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>de</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>shu'ru</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>xin'xi</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>bing'dui</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>shu'ju</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>jin'xing</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>jian'dan</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>de</t>
+    </rPh>
+    <rPh sb="28" eb="29">
+      <t>fen'xi</t>
+    </rPh>
+    <rPh sb="35" eb="36">
+      <t>yuan'shi'shu'ju</t>
+    </rPh>
+    <rPh sb="39" eb="40">
+      <t>he</t>
+    </rPh>
+    <rPh sb="40" eb="41">
+      <t>fen'xi'jie'guo</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC_2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>作为一个用户，可以在设计完问卷之后点击发布按钮，将提醒是否要发布并生成问卷的链接</t>
+    <rPh sb="0" eb="1">
+      <t>zuo'wei</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>yi'ge</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>yong'hu</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>ke'yi</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>zai</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>she'ji</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>wan</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>wen'juan</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>zhi'hou</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>dian'ji</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>fa'bu</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>an'niu</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>jiang</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>ti'xing</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>shi'fou'yao</t>
+    </rPh>
+    <rPh sb="30" eb="31">
+      <t>fa'bu</t>
+    </rPh>
+    <rPh sb="32" eb="33">
+      <t>bing</t>
+    </rPh>
+    <rPh sb="33" eb="34">
+      <t>sheng'cheng</t>
+    </rPh>
+    <rPh sb="35" eb="36">
+      <t>wen'juan</t>
+    </rPh>
+    <rPh sb="37" eb="38">
+      <t>de</t>
+    </rPh>
+    <rPh sb="38" eb="39">
+      <t>lian'jie</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC_2</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -2757,7 +2831,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2792,6 +2866,22 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2810,11 +2900,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2828,9 +2920,11 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="常规 2" xfId="1"/>
+    <cellStyle name="超链接" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="3" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -3132,16 +3226,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="19.625" customWidth="1"/>
-    <col min="2" max="2" width="24.625" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" customWidth="1"/>
     <col min="3" max="3" width="111.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3161,32 +3255,43 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>174</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>175</v>
       </c>
       <c r="C3" t="s">
-        <v>71</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>173</v>
       </c>
       <c r="B4" t="s">
-        <v>73</v>
+        <v>176</v>
       </c>
       <c r="C4" t="s">
-        <v>74</v>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>178</v>
+      </c>
+      <c r="B5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" t="s">
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -3197,22 +3302,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="14.625" customWidth="1"/>
-    <col min="3" max="3" width="31.125" customWidth="1"/>
-    <col min="4" max="4" width="15.125" customWidth="1"/>
-    <col min="5" max="5" width="108.625" customWidth="1"/>
+    <col min="1" max="2" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="36.1640625" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" customWidth="1"/>
+    <col min="5" max="5" width="108.6640625" customWidth="1"/>
     <col min="6" max="6" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3234,665 +3339,682 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" t="s">
         <v>28</v>
       </c>
-      <c r="B2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D2" t="s">
-        <v>30</v>
-      </c>
       <c r="E2" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D4" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="E4" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E5" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D6" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D7" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
         <v>45</v>
       </c>
-      <c r="C8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" t="s">
-        <v>47</v>
-      </c>
       <c r="E8" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E9" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C10" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E10" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="E11" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="E12" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D13" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="E13" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D14" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="E14" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C15" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D15" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="E15" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D16" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E16" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" t="s">
         <v>37</v>
-      </c>
-      <c r="D17" t="s">
-        <v>82</v>
-      </c>
-      <c r="E17" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B18" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" t="s">
         <v>65</v>
       </c>
-      <c r="C18" t="s">
-        <v>67</v>
-      </c>
       <c r="D18" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="E18" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D19" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="E19" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B20" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C20" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D20" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="E20" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C21" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D21" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="E21" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B22" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C22" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D22" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="E22" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B23" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C23" t="s">
+        <v>77</v>
+      </c>
+      <c r="D23" t="s">
+        <v>107</v>
+      </c>
+      <c r="E23" t="s">
         <v>83</v>
-      </c>
-      <c r="D23" t="s">
-        <v>113</v>
-      </c>
-      <c r="E23" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B24" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C24" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D24" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="E24" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B25" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C25" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D25" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="E25" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B26" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C26" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D26" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="E26" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B27" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C27" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D27" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E27" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B28" t="s">
         <v>7</v>
       </c>
       <c r="C28" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="D28" t="s">
-        <v>75</v>
+        <v>107</v>
       </c>
       <c r="E28" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B29" t="s">
         <v>7</v>
       </c>
       <c r="C29" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D29" t="s">
-        <v>75</v>
+        <v>107</v>
       </c>
       <c r="E29" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B30" t="s">
         <v>7</v>
       </c>
       <c r="C30" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="D30" t="s">
-        <v>75</v>
+        <v>107</v>
       </c>
       <c r="E30" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B31" t="s">
         <v>7</v>
       </c>
       <c r="C31" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="D31" t="s">
-        <v>139</v>
+        <v>107</v>
       </c>
       <c r="E31" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B32" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="C32" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="D32" t="s">
-        <v>139</v>
+        <v>107</v>
       </c>
       <c r="E32" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B33" t="s">
-        <v>7</v>
+        <v>184</v>
       </c>
       <c r="C33" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="D33" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="E33" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B34" t="s">
         <v>7</v>
       </c>
       <c r="C34" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="D34" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="E34" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B35" t="s">
         <v>7</v>
       </c>
       <c r="C35" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D35" t="s">
-        <v>148</v>
+        <v>107</v>
       </c>
       <c r="E35" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B36" t="s">
         <v>7</v>
       </c>
       <c r="C36" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="D36" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="E36" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B37" t="s">
         <v>7</v>
       </c>
       <c r="C37" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="D37" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="E37" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B38" t="s">
         <v>7</v>
       </c>
       <c r="C38" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="D38" t="s">
-        <v>155</v>
+        <v>107</v>
       </c>
       <c r="E38" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B39" t="s">
         <v>7</v>
       </c>
       <c r="C39" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D39" t="s">
-        <v>155</v>
+        <v>107</v>
       </c>
       <c r="E39" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B40" t="s">
         <v>7</v>
       </c>
       <c r="C40" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="D40" t="s">
-        <v>155</v>
+        <v>107</v>
       </c>
       <c r="E40" t="s">
-        <v>173</v>
+        <v>167</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A41" t="s">
+        <v>168</v>
+      </c>
+      <c r="B41" t="s">
+        <v>182</v>
+      </c>
+      <c r="C41" t="s">
+        <v>171</v>
+      </c>
+      <c r="D41" t="s">
+        <v>107</v>
+      </c>
+      <c r="E41" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -3907,17 +4029,17 @@
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="15.625" customWidth="1"/>
-    <col min="2" max="2" width="35.875" customWidth="1"/>
-    <col min="3" max="3" width="14.625" customWidth="1"/>
-    <col min="4" max="4" width="19.125" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="35.83203125" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="19.1640625" customWidth="1"/>
     <col min="5" max="5" width="20.5" customWidth="1"/>
-    <col min="6" max="6" width="19.875" customWidth="1"/>
+    <col min="6" max="6" width="19.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.15">
@@ -3942,95 +4064,86 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>112</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D2">
         <v>3</v>
       </c>
       <c r="E2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>118</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="D3">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>125</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>126</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>127</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>128</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="D5">
-        <v>0.5</v>
-      </c>
-      <c r="E5">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>129</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>130</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B7" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -4041,129 +4154,120 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>117</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>71</v>
       </c>
       <c r="C8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D8">
-        <v>0.5</v>
-      </c>
-      <c r="E8">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D9">
         <v>3</v>
       </c>
-      <c r="E9">
-        <v>1.5</v>
-      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>64</v>
+        <v>131</v>
       </c>
       <c r="B10" t="s">
-        <v>80</v>
+        <v>132</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>133</v>
       </c>
       <c r="D10">
-        <v>0.5</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>114</v>
+        <v>134</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>135</v>
       </c>
       <c r="C11" t="s">
-        <v>62</v>
+        <v>133</v>
       </c>
       <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>115</v>
+        <v>42</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D12">
         <v>0.5</v>
       </c>
+      <c r="E12">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
         <v>51</v>
       </c>
-      <c r="C13" t="s">
-        <v>53</v>
-      </c>
       <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="C14" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B15" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="D15">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -4171,64 +4275,64 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B16" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>169</v>
       </c>
       <c r="C17" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="D17">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E17">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B18" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E18">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B19" t="s">
-        <v>176</v>
+        <v>75</v>
       </c>
       <c r="C19" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="D19">
         <v>0.5</v>
@@ -4239,41 +4343,47 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B20" t="s">
         <v>77</v>
       </c>
       <c r="C20" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="D20">
-        <v>1.5</v>
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>0.5</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B21" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" t="s">
         <v>76</v>
       </c>
-      <c r="C21" t="s">
-        <v>75</v>
-      </c>
       <c r="D21">
-        <v>1</v>
+        <v>0.5</v>
+      </c>
+      <c r="E21">
+        <v>0.5</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C22" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D22">
         <v>0.5</v>
@@ -4284,16 +4394,16 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B23" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C23" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E23">
         <v>0.5</v>
@@ -4301,13 +4411,13 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B24" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C24" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D24">
         <v>0.5</v>
@@ -4318,33 +4428,33 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>128</v>
+        <v>33</v>
       </c>
       <c r="B25" t="s">
-        <v>86</v>
+        <v>55</v>
       </c>
       <c r="C25" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D25">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E25">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="B26" t="s">
-        <v>87</v>
+        <v>137</v>
       </c>
       <c r="C26" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D26">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E26">
         <v>0.5</v>
@@ -4352,44 +4462,41 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="B27" t="s">
-        <v>88</v>
+        <v>139</v>
       </c>
       <c r="C27" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D27">
         <v>0.5</v>
       </c>
-      <c r="E27">
-        <v>0.5</v>
-      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="B28" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="C28" t="s">
-        <v>75</v>
+        <v>142</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="B29" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="C29" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -4397,153 +4504,177 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="B30" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="C30" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D30">
+        <v>2</v>
+      </c>
+      <c r="E30">
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>137</v>
+        <v>38</v>
       </c>
       <c r="B31" t="s">
-        <v>138</v>
+        <v>56</v>
       </c>
       <c r="C31" t="s">
-        <v>139</v>
+        <v>53</v>
       </c>
       <c r="D31">
-        <v>2</v>
+        <v>0.5</v>
+      </c>
+      <c r="E31">
+        <v>0.5</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
-        <v>140</v>
+        <v>168</v>
       </c>
       <c r="B32" t="s">
-        <v>141</v>
+        <v>171</v>
       </c>
       <c r="C32" t="s">
-        <v>139</v>
+        <v>172</v>
       </c>
       <c r="D32">
-        <v>3</v>
+        <v>0.5</v>
+      </c>
+      <c r="E32">
+        <v>0.5</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>142</v>
+        <v>40</v>
       </c>
       <c r="B33" t="s">
-        <v>143</v>
+        <v>52</v>
       </c>
       <c r="C33" t="s">
-        <v>82</v>
+        <v>53</v>
       </c>
       <c r="D33">
         <v>1</v>
       </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>144</v>
+        <v>46</v>
       </c>
       <c r="B34" t="s">
-        <v>145</v>
+        <v>19</v>
       </c>
       <c r="C34" t="s">
-        <v>82</v>
+        <v>20</v>
       </c>
       <c r="D34">
-        <v>0.5</v>
+        <v>3</v>
+      </c>
+      <c r="E34">
+        <v>1.5</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
-        <v>146</v>
+        <v>62</v>
       </c>
       <c r="B35" t="s">
-        <v>147</v>
+        <v>74</v>
       </c>
       <c r="C35" t="s">
-        <v>148</v>
+        <v>51</v>
       </c>
       <c r="D35">
         <v>0.5</v>
       </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>149</v>
+        <v>26</v>
       </c>
       <c r="B36" t="s">
-        <v>150</v>
+        <v>64</v>
       </c>
       <c r="C36" t="s">
-        <v>82</v>
+        <v>16</v>
       </c>
       <c r="D36">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="E36">
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
-        <v>151</v>
+        <v>108</v>
       </c>
       <c r="B37" t="s">
-        <v>152</v>
+        <v>22</v>
       </c>
       <c r="C37" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="D37">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
-        <v>153</v>
+        <v>111</v>
       </c>
       <c r="B38" t="s">
-        <v>154</v>
+        <v>23</v>
       </c>
       <c r="C38" t="s">
-        <v>155</v>
+        <v>61</v>
       </c>
       <c r="D38">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="B39" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="C39" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="D39">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="B40" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C40" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="D40">
         <v>1</v>
@@ -4551,22 +4682,22 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
-        <v>174</v>
+        <v>152</v>
       </c>
       <c r="B41" t="s">
-        <v>177</v>
+        <v>153</v>
       </c>
       <c r="C41" t="s">
-        <v>178</v>
+        <v>149</v>
       </c>
       <c r="D41">
-        <v>0.5</v>
-      </c>
-      <c r="E41">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:F41">
+    <sortCondition ref="C1"/>
+  </sortState>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4581,14 +4712,14 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="14.375" customWidth="1"/>
-    <col min="2" max="2" width="17.875" customWidth="1"/>
-    <col min="3" max="3" width="12.875" customWidth="1"/>
-    <col min="4" max="4" width="19.875" customWidth="1"/>
-    <col min="5" max="5" width="18.375" customWidth="1"/>
-    <col min="6" max="6" width="17.375" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" customWidth="1"/>
+    <col min="4" max="4" width="19.83203125" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.15">
@@ -4625,7 +4756,7 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.125" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.1640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
@@ -4661,7 +4792,7 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="19.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">

</xml_diff>

<commit_message>
add function to edit-modal
</commit_message>
<xml_diff>
--- a/doc/迭代开发计划_whyNotDance.xlsx
+++ b/doc/迭代开发计划_whyNotDance.xlsx
@@ -5,11 +5,11 @@
   <workbookPr filterPrivacy="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wang-cy/Desktop/prj1_whynotdance/doc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wang-cy/Documents/软工文档/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Use Cases" sheetId="2" r:id="rId1"/>
@@ -19,6 +19,9 @@
     <sheet name="Sprint 3" sheetId="5" r:id="rId5"/>
     <sheet name="Sprint 4" sheetId="6" r:id="rId6"/>
   </sheets>
+  <definedNames>
+    <definedName name="额">'Product Backlog'!$E$42</definedName>
+  </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -29,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="315">
   <si>
     <t>Feature_ID</t>
   </si>
@@ -2824,6 +2827,2479 @@
   </si>
   <si>
     <t>UC_2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F_41</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>提交填写的问卷信息到数据库</t>
+    <rPh sb="0" eb="1">
+      <t>ti'jiao</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>tian'xie</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>de</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>wen'juan</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>xin'xi</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>dao</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>shu'ju'ku</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>马为之</t>
+    <rPh sb="0" eb="1">
+      <t>ma'wei'zhi</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F_42</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据库更新填写的问卷信息</t>
+    <rPh sb="0" eb="1">
+      <t>shu'ju'ku</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>geng'xin</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>tian'xie'de</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>ween'juan</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>xin'xi</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F_43</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F_44</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>问卷统计页面设计</t>
+    <rPh sb="0" eb="1">
+      <t>wen'juan</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>tong'ji'ye'mian</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>she'ji</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>从后端获取填写者的基本信息显示到列表中</t>
+    <rPh sb="0" eb="1">
+      <t>cong</t>
+    </rPh>
+    <rPh sb="1" eb="2">
+      <t>hou'duan</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>huo'qu</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>tian'xie</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>zhe</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>de</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>ji'ben'xin'xi</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>xian'shi</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>dao</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>lie'biao'zhong</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F_45</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>点击填写者可以查看具体填写的问卷情况</t>
+    <rPh sb="0" eb="1">
+      <t>dian'ji</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>tian'xie'zhe</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>zhe</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>ke'yi</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>cha'kan</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>ju'ti</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>itanxie</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>de</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>wen'jua</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>qing'kuang</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F_46</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据库获得某用户所有某种类型的问卷</t>
+    <rPh sb="0" eb="1">
+      <t>shu'ju'ku</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>huo'de</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>mou'yong'hu</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>suo'you</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>mou'zhong'lei'xing'de</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>wen'juan</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据库根据问卷id获得问卷具体信息</t>
+    <rPh sb="0" eb="1">
+      <t>shu'ju'ku</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>gen'ju</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>wen'juan</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>huo'de</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>wen'juan</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>ju'ti</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>xin'xi</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F_47</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F_48</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户登录的会话控制</t>
+    <rPh sb="0" eb="1">
+      <t>yong'hu</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>deng'lu</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>de</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>hui'hua'kong'zhi</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>页面逻辑与跳转的设计</t>
+    <rPh sb="0" eb="1">
+      <t>ye'mian</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>luo'ji</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>yu</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>tiao'zhuan</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>de</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>she'ji</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户权限与账号关联</t>
+    <rPh sb="0" eb="1">
+      <t>yong'hu</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>quan'xian</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>yu</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>zhang'hao</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>guan'lian</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>一个用户的登录状态需要被保存在会话中，关闭页面后仍记住该状态</t>
+    <rPh sb="0" eb="1">
+      <t>yi'ge</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>yong'hu</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>de</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>deng'lu</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>zhuang't</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>xu'yao</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>bei</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>bao'c</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>zai</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>hui'hua</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>zhong</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>guan'bi</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>ye'm</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>hou</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>reng</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>ji'zhu</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>gai</t>
+    </rPh>
+    <rPh sb="28" eb="29">
+      <t>zhuang't</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>通过各种下拉菜单和超链接将所有页面变为从主页面可达，并且逻辑上相近的页面直接可达</t>
+    <rPh sb="0" eb="1">
+      <t>tong'guo</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>ge'zhong</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>xia'la</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>cai'dan</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>he</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>chao'liang'jie</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>jiang</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>suo'you</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>ye'mian</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>bian'wei</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>cong</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>zhu'ye'm</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>ke'da</t>
+    </rPh>
+    <rPh sb="26" eb="27">
+      <t>bing</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>qie</t>
+    </rPh>
+    <rPh sb="28" eb="29">
+      <t>luo'ji</t>
+    </rPh>
+    <rPh sb="30" eb="31">
+      <t>shang</t>
+    </rPh>
+    <rPh sb="31" eb="32">
+      <t>xiang'jin</t>
+    </rPh>
+    <rPh sb="33" eb="34">
+      <t>de</t>
+    </rPh>
+    <rPh sb="34" eb="35">
+      <t>ye'mian</t>
+    </rPh>
+    <rPh sb="36" eb="37">
+      <t>zhi'jie</t>
+    </rPh>
+    <rPh sb="38" eb="39">
+      <t>ke'da</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>不同的用户的账号通过同一个入口登录，并根据其权限显示不同页面</t>
+    <rPh sb="0" eb="1">
+      <t>bu'tong</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>de</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>yong'hu</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>de</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>zhang'hao</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>tong'guo</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>tong'yi'ge</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>ru'k</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>deng'lu</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>bing</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>gen'j</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>qi</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>quan'x</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>xian'shi</t>
+    </rPh>
+    <rPh sb="26" eb="27">
+      <t>bu'tong</t>
+    </rPh>
+    <rPh sb="28" eb="29">
+      <t>ye'mian</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>管理员页面的设计</t>
+    <rPh sb="0" eb="1">
+      <t>guan'li'y</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ye'm</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>de</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>she'ji</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>管理员公告发布的具体实现</t>
+    <rPh sb="0" eb="1">
+      <t>guan'li'y</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>gong'gao</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>fa'bu</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>de</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>ju'ti</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>shi'xian</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>一个管理员登录后可以通过自己的页面直接发布公告，所有的注册用户和游客都可以接收到公告</t>
+    <rPh sb="0" eb="1">
+      <t>yi'ge</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>guan'li'yuan</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>deng'lu</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>hou</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>ke'yi</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>tong'guo</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>zi'ji</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>de</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>ye'm</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>zhi'jie</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>fa'bu</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>gong'gao</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>suo'you</t>
+    </rPh>
+    <rPh sb="26" eb="27">
+      <t>de</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>zhu'ce</t>
+    </rPh>
+    <rPh sb="29" eb="30">
+      <t>yong'hu</t>
+    </rPh>
+    <rPh sb="31" eb="32">
+      <t>he</t>
+    </rPh>
+    <rPh sb="32" eb="33">
+      <t>you'ke</t>
+    </rPh>
+    <rPh sb="34" eb="35">
+      <t>dou</t>
+    </rPh>
+    <rPh sb="35" eb="36">
+      <t>ke'yi</t>
+    </rPh>
+    <rPh sb="37" eb="38">
+      <t>jie'shou</t>
+    </rPh>
+    <rPh sb="38" eb="39">
+      <t>shou</t>
+    </rPh>
+    <rPh sb="39" eb="40">
+      <t>dao</t>
+    </rPh>
+    <rPh sb="40" eb="41">
+      <t>gong'gao</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户信息和数据库的沟通</t>
+    <rPh sb="0" eb="1">
+      <t>yong'hu</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>xin'xi</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>he</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>shu'ju'k</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>de</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>gou't</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>田文龙</t>
+    <rPh sb="0" eb="1">
+      <t>t'w'l</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>提交时必答题的判断</t>
+    <rPh sb="0" eb="1">
+      <t>ti'jiao's</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>bi'da'ti</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>d</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>pan'd</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>填空题的输入格式判断</t>
+    <rPh sb="0" eb="1">
+      <t>tian'kong'ti</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>d</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>shu'ru</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>ge's</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>pan'd</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>主观题填写格式错误时的提示</t>
+    <rPh sb="0" eb="1">
+      <t>zhu'guan't</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>tian'x</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>ge's</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>cuo'wu</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>s</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>d</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>ti's</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据库保存提交问卷</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据库保存个人信息的修改</t>
+    <rPh sb="0" eb="1">
+      <t>shu'ju'ku</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>bao'cun</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>ge'ren'xin'xi</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>de</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>xiu'gai</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据库获取公告</t>
+    <rPh sb="0" eb="1">
+      <t>shu'ju'ku</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>huo'qu</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>gong'gao</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据库保存对公告的修改</t>
+    <rPh sb="0" eb="1">
+      <t>shu'ju'ku</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>bao'cun</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>dui</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>gong'gao'de</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>xiu'gai</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据库获得所有问卷（管理员）</t>
+    <rPh sb="0" eb="1">
+      <t>shu'ju'ku</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>huo'de</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>suo'you</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>wen'juan</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>guan'li'yuan</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据库根据问卷id获得发布者信息</t>
+    <rPh sb="0" eb="1">
+      <t>shu'ju'ku</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>gen'ju</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>wen'juan</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>huo'de</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>fa'bu'zhe</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>xin'xi</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F_49</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F_50</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F_51</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F_52</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F_53</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F_54</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F_55</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F_56</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F_57</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F_58</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F_59</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F_60</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F_61</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F_62</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F_51</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F_50</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F_49</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>管理员公告在线编辑</t>
+    <rPh sb="0" eb="1">
+      <t>guan'li'yuan</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>gaong'gao</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>zai'xian'bian'ji</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC_3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>作为一个活动参加者，可以简单填写问卷，点击提交后前端将填写情况发送到数据库</t>
+    <rPh sb="0" eb="1">
+      <t>zuo'wei</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>yi'ge</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>huo'dong'can'jia'zhe</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>ke'yi</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>jian'dan</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>tian'xie'wen'juan</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>dian'ji</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>ti'jiao</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>hou</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>qian'duan</t>
+    </rPh>
+    <rPh sb="26" eb="27">
+      <t>jiang</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>tian'xie'qing'kuang</t>
+    </rPh>
+    <rPh sb="31" eb="32">
+      <t>fa'song'dao</t>
+    </rPh>
+    <rPh sb="34" eb="35">
+      <t>shu'ju'ku</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>作为一个活动参加者，点击提交之后数据库能保存填写的信息并更新</t>
+    <rPh sb="0" eb="1">
+      <t>zuo'wei'yi'ge</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>huo'dong'can'yu'zhe</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>jia</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>zhe</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>dian'ji'ti'jiao</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>zhi'hou</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>shu'ju'ku</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>neng</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>bao'cun</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>tian'xie</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>de</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>xin'xi</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>bing</t>
+    </rPh>
+    <rPh sb="28" eb="29">
+      <t>geng'xi</t>
+    </rPh>
+    <rPh sb="29" eb="30">
+      <t>xin</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>作为一个用户，可以进入问卷的统计页面，查看问卷的填写情况</t>
+    <rPh sb="0" eb="1">
+      <t>zuo'wei'yi'ge</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>yong'hu</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>ke'yi'jin'ru</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>wen'juan</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>de</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>tong'ji'ye'mian</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>cha'kan</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>wen'juan'de</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>tian'xie'qing'kuang</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC_4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>前端可以获得某问卷的所有填写者信息并显示到列表中</t>
+    <rPh sb="0" eb="1">
+      <t>qian'duan</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>ke'yi'huo'de</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>mou'wen'juan</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>de</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>suo'you</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>tian'xie</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>zhe</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>xin'xi</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>bing</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>xian'shi</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>dao'lie'biao'zhong</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC_4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>作为一个用户，点击问卷统计页面中的填写者可以查看该填写者填写的具体问卷</t>
+    <rPh sb="0" eb="1">
+      <t>zuo'wei'yi'ge</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>yong'hu</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>dian'ji</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>wen'juan</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>tong'ji</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>ye'mian'zhong'de</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>tian'xie</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>zhe</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>ke'yi'cha'kan</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>gai</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>tian'xie'zhe</t>
+    </rPh>
+    <rPh sb="28" eb="29">
+      <t>tian'xie'de</t>
+    </rPh>
+    <rPh sb="31" eb="32">
+      <t>ju'ti</t>
+    </rPh>
+    <rPh sb="33" eb="34">
+      <t>wen'juan</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC_1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>前端可以获取指定用户指定类型的所有问卷信息</t>
+    <rPh sb="0" eb="1">
+      <t>qian'duan</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>ke'yi'huo'qu</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>zhi'ding'yong'hu</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>zhi'ding</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>de</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>suo'you</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>wen'juan</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>xin'xi</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC_1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>前端可以根据问卷id获取问卷详细信息并据此进入修改问卷页面</t>
+    <rPh sb="0" eb="1">
+      <t>qian'duan</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>ke'yi</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>gen'ju</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>wen'juan</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>huo'qu</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>wen'juan</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>xiang'xi'xin'xi</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>bing</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>ju'ci</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>jin'ru</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>xiu'gai</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>wen'juan</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>ye'mian</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>作为一个管理员，登录后可以查看所有用户信息和所有问卷信息</t>
+    <rPh sb="0" eb="1">
+      <t>zuo'wei</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>yi'ge</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>deng'lu</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>hou</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>ke'yi</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>cha'kan</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>suo'you</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>yong'hu</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>xin'xi</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>he</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>suo'you</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>wen'juan</t>
+    </rPh>
+    <rPh sb="26" eb="27">
+      <t>xin'xi</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>修改用户信息和数据库交互</t>
+    <rPh sb="0" eb="1">
+      <t>xiu'gai</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>yong'hu'xin'xi</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>he</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>shu'ju'ku</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>jiao'hu</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC_3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>作为一个活动参加者，在没有答必答题的情况下点击提交或提示信息</t>
+    <rPh sb="0" eb="1">
+      <t>zuo'wei'yi'ge</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ge</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>huo'dong</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>can'jia'zhe</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>zai</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>mei'you</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>da</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>bi'da'ti</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>de</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>qing'kuang'xia</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>dian'ji</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>ti'jiao</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>huo'ti'shi</t>
+    </rPh>
+    <rPh sb="28" eb="29">
+      <t>xin'xi</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>作为一个活动参加者，填空题输入格式错误会给出提示</t>
+    <rPh sb="0" eb="1">
+      <t>zuo'wei'yi'ge</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>huo'dong'can'jia'zhe</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>tian'kong'ti</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>shu'ru</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>ge'shi</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>cuo'weu</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>hui</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>gei'chu'ti'shi</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC_3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>作为一个活动参加者，前端判断填空题输入格式是否符合要求</t>
+    <rPh sb="0" eb="1">
+      <t>zuo'wei'yi'ge</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>huo'dong'can'jia'zhe</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>qian'duan</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>pan'duan</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>tian'kong'ti</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>shu'ru</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>ge'shi</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>shi'fou</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>fu'he'yao'qiu</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC_1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据库可以保存用户对用户信息的修改</t>
+    <rPh sb="0" eb="1">
+      <t>shu'ju'ku</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ke'yi</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>bao'cun</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>yong'hu</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>dui</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>yong'hu</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>xin'xi</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>de</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>xiu'gai</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC_1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>前端可以从数据库获取公告的内容</t>
+    <rPh sb="0" eb="1">
+      <t>qian'duan</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>ke'yi'cong</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>shu'ju'ku</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>huo'qu</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>gong'gao</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>de</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>nei'rong</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据库可以保存对于公告的修改并更新</t>
+    <rPh sb="0" eb="1">
+      <t>shu'ju'ku</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ke'yi'bao'cun</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>dui'yu</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>gong'gao</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>de</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>xiu'gai</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>bing'geng'xin</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>前端可以从数据库获得所有已发布的问卷</t>
+    <rPh sb="0" eb="1">
+      <t>qian'duan</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>ke'yi'xong</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>cong</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>shu'ju'ku</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>huo'de</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>suo'you</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>yi'fa'bu</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>de</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>wen'juan</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>在管理员页面可以显示左右发布的报名及其发布者</t>
+    <rPh sb="0" eb="1">
+      <t>zai</t>
+    </rPh>
+    <rPh sb="1" eb="2">
+      <t>guan'li'yuan</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>ye'mian</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>ke'yi'xian'shi</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>zuo'you</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>fa'bu'de</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>bao'ming</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>ji</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>qi</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>fa'bu'zhe</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>作为一个管理员，可以在线编辑管理员公告并在页面上实时更新</t>
+    <rPh sb="0" eb="1">
+      <t>zuo'wei'yi'ge</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>guan'li'yuan</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>ke'yi'zai</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>zai'xian'bian'ji</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>guan'li'yuan'gong'gao</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>bing</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>zai</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>ye'mian</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>shang</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>shi'shi</t>
+    </rPh>
+    <rPh sb="26" eb="27">
+      <t>geng'xin</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F_43</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>徐子南</t>
+    <rPh sb="0" eb="1">
+      <t>xu'zi'nna</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>管理员公告在线编辑</t>
+    <rPh sb="0" eb="1">
+      <t>guan'li'yuan</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>gong'gao'bian'ji</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>zai'xian</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F_63</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>点击统计信息选择要查看的问卷</t>
+    <rPh sb="0" eb="1">
+      <t>dian'ji</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>tong'ji'xin'xi</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>xuan'ze</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>yao</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>cha'kan</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>de</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>wen'juan</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F_64</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出所有填写者的ip等信息</t>
+    <rPh sb="0" eb="1">
+      <t>lie'chu</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>suo'you</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>tian'xie</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>zhe</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>de</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>deng</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>xin'xi</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F_65</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看问卷所有题目的统计信息</t>
+    <rPh sb="0" eb="1">
+      <t>cha'kan</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>wen'juan</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>suo'you'ti'mu</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>de</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>tong'ji'xin'xi</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC_4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC_4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC_4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>马为之</t>
+    <rPh sb="0" eb="1">
+      <t>ma'we'zhi</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>作为一个用户，可以点击左边栏的统计信息，选择要查看的问卷</t>
+    <rPh sb="0" eb="1">
+      <t>zuo'wei'yi'ge</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>yong'hu</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>ke'yi</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>dian'ji</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>zuo'bian'lan</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>de</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>tong'ji'xin'xi</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>xuan'ze</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>yao'cha'kan</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>de</t>
+    </rPh>
+    <rPh sb="26" eb="27">
+      <t>wen'juan</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>作为一个用户，选择要查看统计的问卷后显示所有填写者信息，包括ip、时间等</t>
+    <rPh sb="0" eb="1">
+      <t>zuo'wei'yi'ge</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>yong'hu</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>xuan'ze</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>yao'cha'kan</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>tong'ji</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>de</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>wen'juan</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>hou</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>xian'shi</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>suo'you</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>tian'xie'zhe</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>xin'xi</t>
+    </rPh>
+    <rPh sb="28" eb="29">
+      <t>bao'kuo</t>
+    </rPh>
+    <rPh sb="33" eb="34">
+      <t>shi'jian</t>
+    </rPh>
+    <rPh sb="35" eb="36">
+      <t>deng</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>作为一个用户，选择要查看数据的问卷后显示所有题目的统计信息，以表格呈现</t>
+    <rPh sb="0" eb="1">
+      <t>zuo'wei'yi'ge</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>yong'hu</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>xuan'ze</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>yao'cha'kan</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>shu'ju</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>de</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>wen'juan</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>hou</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>xian'shi</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>suo'you</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>ti'mu</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>de</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>tong'ji'xin'xi</t>
+    </rPh>
+    <rPh sb="30" eb="31">
+      <t>yi</t>
+    </rPh>
+    <rPh sb="31" eb="32">
+      <t>biao'ge</t>
+    </rPh>
+    <rPh sb="33" eb="34">
+      <t>cheng'xian</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F_66</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>首页和所有报名页面快捷按钮跳转实现</t>
+    <rPh sb="0" eb="1">
+      <t>shou'ye</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>he</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>suo'you</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>bao'ming</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>ye'mian</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>kuai'jie</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>an'niu</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>tiao'zhuan</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>shi'xian</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F_67</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>同页面多张可排序表格功能调整</t>
+    <rPh sb="0" eb="1">
+      <t>tong'ye'mian</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>duo'zhang</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>ke'pai'xu'biao'ge</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>gong'neng</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>tiao'zheng</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC_1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC_4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>作为一个已登录用户，可以在首页和所有报名页面点击操作展开下拉菜单，并通过点击查看相应问卷的各种信息、对问卷进行操作</t>
+    <rPh sb="0" eb="1">
+      <t>zuo'wei'yi'ge</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>yi'deng'lu</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>yong'hu</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>ke'yi</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>zai</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>shou'y</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>he</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>suo'you'bao'ming</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>ye'mian</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>dian'ji</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>cao'zuo</t>
+    </rPh>
+    <rPh sb="26" eb="27">
+      <t>zhan'kai</t>
+    </rPh>
+    <rPh sb="28" eb="29">
+      <t>xia'la</t>
+    </rPh>
+    <rPh sb="30" eb="31">
+      <t>cai'dan</t>
+    </rPh>
+    <rPh sb="33" eb="34">
+      <t>bing'tong'guo</t>
+    </rPh>
+    <rPh sb="36" eb="37">
+      <t>dian'ji</t>
+    </rPh>
+    <rPh sb="38" eb="39">
+      <t>cha'kan</t>
+    </rPh>
+    <rPh sb="40" eb="41">
+      <t>xiang'ying</t>
+    </rPh>
+    <rPh sb="42" eb="43">
+      <t>wen'juan</t>
+    </rPh>
+    <rPh sb="44" eb="45">
+      <t>de</t>
+    </rPh>
+    <rPh sb="45" eb="46">
+      <t>ge'zhong</t>
+    </rPh>
+    <rPh sb="47" eb="48">
+      <t>xin'xi</t>
+    </rPh>
+    <rPh sb="50" eb="51">
+      <t>dui</t>
+    </rPh>
+    <rPh sb="51" eb="52">
+      <t>wen'juan</t>
+    </rPh>
+    <rPh sb="53" eb="54">
+      <t>jin'xing</t>
+    </rPh>
+    <rPh sb="55" eb="56">
+      <t>cao'zuo</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>解决同一页面显示多张表格时，排序搜索功能互相错位问题</t>
+    <rPh sb="0" eb="1">
+      <t>jie'jue</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>tong</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>yi</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>ye'mian</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>xian'shi</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>duo'zhang</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>biao'ge</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>shi</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>pai'xu</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>sou'suo'gong'neng</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>hu'xiang</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>cuo'wei</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>wen'ti</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F_68</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>统计页面单选题数据的图形化表示</t>
+    <rPh sb="0" eb="1">
+      <t>tong'ji'ye'mian</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>dan'xuan'ti</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>shu'ju</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>de</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>tu'xing'hua</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>biao'shi</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F_69</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>设计问卷页面排序题设计</t>
+    <rPh sb="0" eb="1">
+      <t>she'ji'ye'mian</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>wen'juan</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>pai'xu</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>ti</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>she'ji</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F_70</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>设计页面排序题在线编辑</t>
+    <rPh sb="0" eb="1">
+      <t>she'ji'ye'mian</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>pai'xu'ti</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>zai'xian'bian'ji</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC_4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>作为一个用户，可以在数据统计页面查看单选题数据的图形化表示</t>
+    <rPh sb="0" eb="1">
+      <t>zuo'wei'yi'ge</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>yong'hu</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>ke'yi</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>zai</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>shu'ju'tong'ji</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>ye'mian</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>cha'kan</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>dan'xuan'ti</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>shu'ju</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>de</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>tu'xing'hua</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>biao'shi</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>作为一个用户，可以在设计问卷页面点击排序题向问卷中添加排序题</t>
+    <rPh sb="0" eb="1">
+      <t>zuo'wei'yi'ge</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>yong'hu</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>ke'yi'zai</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>zai</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>she'ji</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>wen'juan</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>ye'mian</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>dian'ji</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>pai'xu</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>ti</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>xiang</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>wen'juan'zhong'tian'jia</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>pai'xu'ti</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>作为一个用户，可以在线编辑排序题，页面实时更新，并向后端发送消息</t>
+    <rPh sb="0" eb="1">
+      <t>zuo'wei'yi'ge'yong'hu</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>ke'yi'zai'xian</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>bian'ji</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>pai'xu'ti</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>ye'mian</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>shi'shi</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>geng'xin</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>bing</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>xiang</t>
+    </rPh>
+    <rPh sb="26" eb="27">
+      <t>hou'duan</t>
+    </rPh>
+    <rPh sb="28" eb="29">
+      <t>fa'song</t>
+    </rPh>
+    <rPh sb="30" eb="31">
+      <t>xiao'xi</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F_71</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户请求非法url时的重定向</t>
+    <rPh sb="0" eb="1">
+      <t>yong'hu</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>qing'qiu</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>fei'fa</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>shi</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>de</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>chong'ding'x</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F_72</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>管理员界面查看信息的表格移植</t>
+    <rPh sb="0" eb="1">
+      <t>guan'li'y</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>jie'm</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>cha'kan</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>xin'xi</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>de</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>biao'ge</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>yi'zhi</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>游客界面问卷填写功能的移植</t>
+    <rPh sb="0" eb="1">
+      <t>you'ke</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>jie'm</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>wen'juan</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>tian'xie</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>gong'neng</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>de</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>yi'zhi</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>游客页面问卷设计</t>
+    <rPh sb="0" eb="1">
+      <t>you'ke</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>ye'm</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>wen'juan</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>she'ji</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>ji</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>非注册用户可以再不登录的情况下发布问卷</t>
+    <rPh sb="0" eb="1">
+      <t>fei'zhu'ce</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>yong'hu</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>ke'yi</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>zai</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>bu'deng'lu</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>de</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>qing'k</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>xia</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>fa'bu</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>wen'juan</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>管理员信息查看功能的实现</t>
+    <rPh sb="0" eb="1">
+      <t>guan'li'y</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>xin'xi</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>cha'kan</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>gong'neg</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>de</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>shi'xian</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>作为一个管理员，登录后可以查看所有用户和所有问卷的信息</t>
+    <rPh sb="0" eb="1">
+      <t>zuo'wei</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>yi'ge</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>guan'li'y</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>deng'lu</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>hou</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>ke'yi</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>cha'kan</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>suo'you</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>yong'hu</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>he</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>suo'you</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>wen'juan</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>de</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>xin'xi</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户请求非法URL时的重定向</t>
+    <rPh sb="0" eb="1">
+      <t>yong'hu</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>qing'qiu</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>fei'fa</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>shi</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>de</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>chong'ding'x</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户如果直接通过url访问不符合权限的界面会自动跳转到登录界面</t>
+    <rPh sb="0" eb="1">
+      <t>yong'hu</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>ru'guo</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>zhi'jie</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>tong'guo</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>fang'wen</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>bu'fu'he</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>quan'xian</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>de</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>jie'm</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>hui</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>zi'dong</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>tiao'zhuan</t>
+    </rPh>
+    <rPh sb="26" eb="27">
+      <t>dao</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>deng'lu</t>
+    </rPh>
+    <rPh sb="29" eb="30">
+      <t>jie'm</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F_73</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据库保存对于题目的编辑</t>
+    <rPh sb="0" eb="1">
+      <t>shu'ju'ku</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>bao'cun</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>dui'yu</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>ti'mu</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>de</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>bian'ji</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F_74</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据库可以保存对于题目内容的编辑并保存</t>
+    <rPh sb="0" eb="1">
+      <t>shu'ju'ku</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ke'yi'bao'cun</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>dui'yu</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>ti'mu</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>nei'rong</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>de</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>bian'ji</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>bing</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>bao'cun</t>
+    </rPh>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -3302,10 +5778,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="B52" zoomScale="125" workbookViewId="0">
+      <selection activeCell="E75" sqref="E75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -3549,7 +6025,7 @@
         <v>63</v>
       </c>
       <c r="C14" t="s">
-        <v>23</v>
+        <v>215</v>
       </c>
       <c r="D14" t="s">
         <v>107</v>
@@ -4015,6 +6491,584 @@
       </c>
       <c r="E41" t="s">
         <v>183</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A42" t="s">
+        <v>185</v>
+      </c>
+      <c r="B42" t="s">
+        <v>239</v>
+      </c>
+      <c r="C42" t="s">
+        <v>186</v>
+      </c>
+      <c r="D42" t="s">
+        <v>187</v>
+      </c>
+      <c r="E42" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A43" t="s">
+        <v>188</v>
+      </c>
+      <c r="B43" t="s">
+        <v>239</v>
+      </c>
+      <c r="C43" t="s">
+        <v>189</v>
+      </c>
+      <c r="D43" t="s">
+        <v>187</v>
+      </c>
+      <c r="E43" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A44" t="s">
+        <v>191</v>
+      </c>
+      <c r="B44" t="s">
+        <v>178</v>
+      </c>
+      <c r="C44" t="s">
+        <v>192</v>
+      </c>
+      <c r="D44" t="s">
+        <v>187</v>
+      </c>
+      <c r="E44" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A45" t="s">
+        <v>194</v>
+      </c>
+      <c r="B45" t="s">
+        <v>243</v>
+      </c>
+      <c r="C45" t="s">
+        <v>193</v>
+      </c>
+      <c r="D45" t="s">
+        <v>187</v>
+      </c>
+      <c r="E45" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A46" t="s">
+        <v>196</v>
+      </c>
+      <c r="B46" t="s">
+        <v>245</v>
+      </c>
+      <c r="C46" t="s">
+        <v>195</v>
+      </c>
+      <c r="D46" t="s">
+        <v>76</v>
+      </c>
+      <c r="E46" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A47" t="s">
+        <v>199</v>
+      </c>
+      <c r="B47" t="s">
+        <v>247</v>
+      </c>
+      <c r="C47" t="s">
+        <v>197</v>
+      </c>
+      <c r="D47" t="s">
+        <v>187</v>
+      </c>
+      <c r="E47" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A48" t="s">
+        <v>200</v>
+      </c>
+      <c r="B48" t="s">
+        <v>249</v>
+      </c>
+      <c r="C48" t="s">
+        <v>198</v>
+      </c>
+      <c r="D48" t="s">
+        <v>187</v>
+      </c>
+      <c r="E48" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A49" t="s">
+        <v>221</v>
+      </c>
+      <c r="B49" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49" t="s">
+        <v>201</v>
+      </c>
+      <c r="D49" t="s">
+        <v>187</v>
+      </c>
+      <c r="E49" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A50" t="s">
+        <v>222</v>
+      </c>
+      <c r="B50" t="s">
+        <v>7</v>
+      </c>
+      <c r="C50" t="s">
+        <v>202</v>
+      </c>
+      <c r="D50" t="s">
+        <v>187</v>
+      </c>
+      <c r="E50" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A51" t="s">
+        <v>223</v>
+      </c>
+      <c r="B51" t="s">
+        <v>7</v>
+      </c>
+      <c r="C51" t="s">
+        <v>203</v>
+      </c>
+      <c r="D51" t="s">
+        <v>187</v>
+      </c>
+      <c r="E51" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A52" t="s">
+        <v>224</v>
+      </c>
+      <c r="B52" t="s">
+        <v>7</v>
+      </c>
+      <c r="C52" t="s">
+        <v>207</v>
+      </c>
+      <c r="D52" t="s">
+        <v>187</v>
+      </c>
+      <c r="E52" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A53" t="s">
+        <v>225</v>
+      </c>
+      <c r="B53" t="s">
+        <v>7</v>
+      </c>
+      <c r="C53" t="s">
+        <v>208</v>
+      </c>
+      <c r="D53" t="s">
+        <v>187</v>
+      </c>
+      <c r="E53" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A54" t="s">
+        <v>226</v>
+      </c>
+      <c r="B54" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54" t="s">
+        <v>210</v>
+      </c>
+      <c r="D54" t="s">
+        <v>69</v>
+      </c>
+      <c r="E54" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A55" t="s">
+        <v>227</v>
+      </c>
+      <c r="B55" t="s">
+        <v>253</v>
+      </c>
+      <c r="C55" t="s">
+        <v>212</v>
+      </c>
+      <c r="D55" t="s">
+        <v>76</v>
+      </c>
+      <c r="E55" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A56" t="s">
+        <v>228</v>
+      </c>
+      <c r="B56" t="s">
+        <v>253</v>
+      </c>
+      <c r="C56" t="s">
+        <v>213</v>
+      </c>
+      <c r="D56" t="s">
+        <v>187</v>
+      </c>
+      <c r="E56" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A57" t="s">
+        <v>229</v>
+      </c>
+      <c r="B57" t="s">
+        <v>256</v>
+      </c>
+      <c r="C57" t="s">
+        <v>214</v>
+      </c>
+      <c r="D57" t="s">
+        <v>187</v>
+      </c>
+      <c r="E57" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A58" t="s">
+        <v>230</v>
+      </c>
+      <c r="B58" t="s">
+        <v>258</v>
+      </c>
+      <c r="C58" t="s">
+        <v>216</v>
+      </c>
+      <c r="D58" t="s">
+        <v>187</v>
+      </c>
+      <c r="E58" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A59" t="s">
+        <v>231</v>
+      </c>
+      <c r="B59" t="s">
+        <v>260</v>
+      </c>
+      <c r="C59" t="s">
+        <v>217</v>
+      </c>
+      <c r="D59" t="s">
+        <v>187</v>
+      </c>
+      <c r="E59" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A60" t="s">
+        <v>232</v>
+      </c>
+      <c r="B60" t="s">
+        <v>7</v>
+      </c>
+      <c r="C60" t="s">
+        <v>218</v>
+      </c>
+      <c r="D60" t="s">
+        <v>187</v>
+      </c>
+      <c r="E60" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A61" t="s">
+        <v>233</v>
+      </c>
+      <c r="B61" t="s">
+        <v>258</v>
+      </c>
+      <c r="C61" t="s">
+        <v>219</v>
+      </c>
+      <c r="D61" t="s">
+        <v>187</v>
+      </c>
+      <c r="E61" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A62" t="s">
+        <v>234</v>
+      </c>
+      <c r="B62" t="s">
+        <v>7</v>
+      </c>
+      <c r="C62" t="s">
+        <v>220</v>
+      </c>
+      <c r="D62" t="s">
+        <v>187</v>
+      </c>
+      <c r="E62" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A63" t="s">
+        <v>190</v>
+      </c>
+      <c r="B63" t="s">
+        <v>7</v>
+      </c>
+      <c r="C63" t="s">
+        <v>238</v>
+      </c>
+      <c r="D63" t="s">
+        <v>133</v>
+      </c>
+      <c r="E63" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A64" t="s">
+        <v>269</v>
+      </c>
+      <c r="B64" t="s">
+        <v>275</v>
+      </c>
+      <c r="C64" t="s">
+        <v>270</v>
+      </c>
+      <c r="D64" t="s">
+        <v>278</v>
+      </c>
+      <c r="E64" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A65" t="s">
+        <v>271</v>
+      </c>
+      <c r="B65" t="s">
+        <v>276</v>
+      </c>
+      <c r="C65" t="s">
+        <v>272</v>
+      </c>
+      <c r="D65" t="s">
+        <v>187</v>
+      </c>
+      <c r="E65" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A66" t="s">
+        <v>273</v>
+      </c>
+      <c r="B66" t="s">
+        <v>277</v>
+      </c>
+      <c r="C66" t="s">
+        <v>274</v>
+      </c>
+      <c r="D66" t="s">
+        <v>187</v>
+      </c>
+      <c r="E66" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A67" t="s">
+        <v>282</v>
+      </c>
+      <c r="B67" t="s">
+        <v>286</v>
+      </c>
+      <c r="C67" t="s">
+        <v>283</v>
+      </c>
+      <c r="D67" t="s">
+        <v>76</v>
+      </c>
+      <c r="E67" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A68" t="s">
+        <v>284</v>
+      </c>
+      <c r="B68" t="s">
+        <v>287</v>
+      </c>
+      <c r="C68" t="s">
+        <v>285</v>
+      </c>
+      <c r="D68" t="s">
+        <v>76</v>
+      </c>
+      <c r="E68" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A69" t="s">
+        <v>290</v>
+      </c>
+      <c r="B69" t="s">
+        <v>296</v>
+      </c>
+      <c r="C69" t="s">
+        <v>291</v>
+      </c>
+      <c r="D69" t="s">
+        <v>187</v>
+      </c>
+      <c r="E69" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A70" t="s">
+        <v>292</v>
+      </c>
+      <c r="B70" t="s">
+        <v>247</v>
+      </c>
+      <c r="C70" t="s">
+        <v>293</v>
+      </c>
+      <c r="D70" t="s">
+        <v>187</v>
+      </c>
+      <c r="E70" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A71" t="s">
+        <v>294</v>
+      </c>
+      <c r="B71" t="s">
+        <v>247</v>
+      </c>
+      <c r="C71" t="s">
+        <v>295</v>
+      </c>
+      <c r="D71" t="s">
+        <v>187</v>
+      </c>
+      <c r="E71" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A72" t="s">
+        <v>300</v>
+      </c>
+      <c r="B72" t="s">
+        <v>154</v>
+      </c>
+      <c r="C72" t="s">
+        <v>305</v>
+      </c>
+      <c r="D72" t="s">
+        <v>187</v>
+      </c>
+      <c r="E72" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A73" t="s">
+        <v>302</v>
+      </c>
+      <c r="B73" t="s">
+        <v>286</v>
+      </c>
+      <c r="C73" t="s">
+        <v>307</v>
+      </c>
+      <c r="D73" t="s">
+        <v>187</v>
+      </c>
+      <c r="E73" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A74" t="s">
+        <v>311</v>
+      </c>
+      <c r="B74" t="s">
+        <v>286</v>
+      </c>
+      <c r="C74" t="s">
+        <v>309</v>
+      </c>
+      <c r="D74" t="s">
+        <v>76</v>
+      </c>
+      <c r="E74" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A75" t="s">
+        <v>313</v>
+      </c>
+      <c r="B75" t="s">
+        <v>247</v>
+      </c>
+      <c r="C75" t="s">
+        <v>312</v>
+      </c>
+      <c r="D75" t="s">
+        <v>278</v>
+      </c>
+      <c r="E75" t="s">
+        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -4026,10 +7080,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView topLeftCell="A20" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -4092,6 +7146,9 @@
       <c r="D3">
         <v>1</v>
       </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
@@ -4106,6 +7163,9 @@
       <c r="D4">
         <v>1</v>
       </c>
+      <c r="E4">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
@@ -4120,6 +7180,9 @@
       <c r="D5">
         <v>1</v>
       </c>
+      <c r="E5">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
@@ -4134,6 +7197,9 @@
       <c r="D6">
         <v>1</v>
       </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
@@ -4165,6 +7231,9 @@
       <c r="D8">
         <v>1.5</v>
       </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
@@ -4207,6 +7276,9 @@
       <c r="D11">
         <v>3</v>
       </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
@@ -4238,6 +7310,9 @@
       <c r="D13">
         <v>0.5</v>
       </c>
+      <c r="E13">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
@@ -4473,6 +7548,9 @@
       <c r="D27">
         <v>0.5</v>
       </c>
+      <c r="E27">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
@@ -4487,6 +7565,9 @@
       <c r="D28">
         <v>0.5</v>
       </c>
+      <c r="E28">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
@@ -4501,6 +7582,9 @@
       <c r="D29">
         <v>1</v>
       </c>
+      <c r="E29">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
@@ -4651,6 +7735,9 @@
       <c r="D38">
         <v>1</v>
       </c>
+      <c r="E38">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
@@ -4665,6 +7752,9 @@
       <c r="D39">
         <v>0.5</v>
       </c>
+      <c r="E39">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
@@ -4679,6 +7769,9 @@
       <c r="D40">
         <v>1</v>
       </c>
+      <c r="E40">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
@@ -4692,6 +7785,77 @@
       </c>
       <c r="D41">
         <v>1</v>
+      </c>
+      <c r="E41">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A42" t="s">
+        <v>237</v>
+      </c>
+      <c r="B42" t="s">
+        <v>201</v>
+      </c>
+      <c r="C42" t="s">
+        <v>69</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A43" t="s">
+        <v>236</v>
+      </c>
+      <c r="B43" t="s">
+        <v>202</v>
+      </c>
+      <c r="C43" t="s">
+        <v>69</v>
+      </c>
+      <c r="D43">
+        <v>0.5</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A44" t="s">
+        <v>235</v>
+      </c>
+      <c r="B44" t="s">
+        <v>203</v>
+      </c>
+      <c r="C44" t="s">
+        <v>69</v>
+      </c>
+      <c r="D44">
+        <v>0.5</v>
+      </c>
+      <c r="E44">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A45" t="s">
+        <v>266</v>
+      </c>
+      <c r="B45" t="s">
+        <v>268</v>
+      </c>
+      <c r="C45" t="s">
+        <v>211</v>
+      </c>
+      <c r="D45">
+        <v>0.5</v>
+      </c>
+      <c r="E45">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -4706,16 +7870,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView topLeftCell="A3" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="14.33203125" customWidth="1"/>
-    <col min="2" max="2" width="17.83203125" customWidth="1"/>
+    <col min="2" max="2" width="38" customWidth="1"/>
     <col min="3" max="3" width="12.83203125" customWidth="1"/>
     <col min="4" max="4" width="19.83203125" customWidth="1"/>
     <col min="5" max="5" width="18.33203125" customWidth="1"/>
@@ -4740,6 +7904,474 @@
       </c>
       <c r="F1" s="3" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B4" t="s">
+        <v>192</v>
+      </c>
+      <c r="C4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>194</v>
+      </c>
+      <c r="B5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>196</v>
+      </c>
+      <c r="B6" t="s">
+        <v>195</v>
+      </c>
+      <c r="C6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>199</v>
+      </c>
+      <c r="B7" t="s">
+        <v>197</v>
+      </c>
+      <c r="C7" t="s">
+        <v>149</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>200</v>
+      </c>
+      <c r="B8" t="s">
+        <v>198</v>
+      </c>
+      <c r="C8" t="s">
+        <v>149</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>224</v>
+      </c>
+      <c r="B9" t="s">
+        <v>207</v>
+      </c>
+      <c r="C9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>225</v>
+      </c>
+      <c r="B10" t="s">
+        <v>208</v>
+      </c>
+      <c r="C10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>226</v>
+      </c>
+      <c r="B11" t="s">
+        <v>210</v>
+      </c>
+      <c r="C11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>227</v>
+      </c>
+      <c r="B12" t="s">
+        <v>212</v>
+      </c>
+      <c r="C12" t="s">
+        <v>133</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>228</v>
+      </c>
+      <c r="B13" t="s">
+        <v>213</v>
+      </c>
+      <c r="C13" t="s">
+        <v>133</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>229</v>
+      </c>
+      <c r="B14" t="s">
+        <v>214</v>
+      </c>
+      <c r="C14" t="s">
+        <v>133</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A15" t="s">
+        <v>230</v>
+      </c>
+      <c r="B15" t="s">
+        <v>216</v>
+      </c>
+      <c r="C15" t="s">
+        <v>149</v>
+      </c>
+      <c r="D15">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
+        <v>231</v>
+      </c>
+      <c r="B16" t="s">
+        <v>217</v>
+      </c>
+      <c r="C16" t="s">
+        <v>149</v>
+      </c>
+      <c r="D16">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>232</v>
+      </c>
+      <c r="B17" t="s">
+        <v>218</v>
+      </c>
+      <c r="C17" t="s">
+        <v>267</v>
+      </c>
+      <c r="D17">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>233</v>
+      </c>
+      <c r="B18" t="s">
+        <v>219</v>
+      </c>
+      <c r="C18" t="s">
+        <v>149</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
+        <v>234</v>
+      </c>
+      <c r="B19" t="s">
+        <v>220</v>
+      </c>
+      <c r="C19" t="s">
+        <v>149</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
+        <v>269</v>
+      </c>
+      <c r="B20" t="s">
+        <v>270</v>
+      </c>
+      <c r="C20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D20">
+        <v>0.5</v>
+      </c>
+      <c r="E20">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A21" t="s">
+        <v>271</v>
+      </c>
+      <c r="B21" t="s">
+        <v>272</v>
+      </c>
+      <c r="C21" t="s">
+        <v>76</v>
+      </c>
+      <c r="D21">
+        <v>0.5</v>
+      </c>
+      <c r="E21">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A22" t="s">
+        <v>273</v>
+      </c>
+      <c r="B22" t="s">
+        <v>274</v>
+      </c>
+      <c r="C22" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A23" t="s">
+        <v>282</v>
+      </c>
+      <c r="B23" t="s">
+        <v>283</v>
+      </c>
+      <c r="C23" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A24" t="s">
+        <v>284</v>
+      </c>
+      <c r="B24" t="s">
+        <v>285</v>
+      </c>
+      <c r="C24" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A25" t="s">
+        <v>290</v>
+      </c>
+      <c r="B25" t="s">
+        <v>291</v>
+      </c>
+      <c r="C25" t="s">
+        <v>76</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A26" t="s">
+        <v>292</v>
+      </c>
+      <c r="B26" t="s">
+        <v>293</v>
+      </c>
+      <c r="C26" t="s">
+        <v>76</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A27" t="s">
+        <v>294</v>
+      </c>
+      <c r="B27" t="s">
+        <v>295</v>
+      </c>
+      <c r="C27" t="s">
+        <v>76</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A28" t="s">
+        <v>300</v>
+      </c>
+      <c r="B28" t="s">
+        <v>301</v>
+      </c>
+      <c r="C28" t="s">
+        <v>69</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A29" t="s">
+        <v>302</v>
+      </c>
+      <c r="B29" t="s">
+        <v>303</v>
+      </c>
+      <c r="C29" t="s">
+        <v>69</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A30" t="s">
+        <v>311</v>
+      </c>
+      <c r="B30" t="s">
+        <v>304</v>
+      </c>
+      <c r="C30" t="s">
+        <v>69</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A31" t="s">
+        <v>313</v>
+      </c>
+      <c r="B31" t="s">
+        <v>312</v>
+      </c>
+      <c r="C31" t="s">
+        <v>149</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>